<commit_message>
working on exporting to excel
</commit_message>
<xml_diff>
--- a/AssignmentList.xlsx
+++ b/AssignmentList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Java</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>Thu May 02 16:20:00 CDT 2019</t>
+  </si>
+  <si>
+    <t>Essay</t>
+  </si>
+  <si>
+    <t>Fri May 10 00:00:00 CDT 2019</t>
   </si>
 </sst>
 </file>
@@ -80,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -128,6 +134,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1234.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
working on google calendar and gui
</commit_message>
<xml_diff>
--- a/AssignmentList.xlsx
+++ b/AssignmentList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Java</t>
   </si>
@@ -32,16 +32,19 @@
     <t>Sat May 04 00:00:00 CDT 2019</t>
   </si>
   <si>
-    <t>Lab 11 gui and database</t>
-  </si>
-  <si>
-    <t>Thu May 02 16:20:00 CDT 2019</t>
-  </si>
-  <si>
     <t>Essay</t>
   </si>
   <si>
     <t>Fri May 10 00:00:00 CDT 2019</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>Chapter 10 questions</t>
+  </si>
+  <si>
+    <t>Mon May 06 13:54:27 CDT 2019</t>
   </si>
 </sst>
 </file>
@@ -122,10 +125,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>2545.0</v>
+        <v>1234.0</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -136,16 +139,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>1234.0</v>
+        <v>3423.0</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>